<commit_message>
add new generated data. 13970514
</commit_message>
<xml_diff>
--- a/logs_csv/pdfs/model_common_diagrams.xlsx
+++ b/logs_csv/pdfs/model_common_diagrams.xlsx
@@ -21,24 +21,9 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="6">
   <si>
     <t>epoch</t>
-  </si>
-  <si>
-    <t>loss_model1</t>
-  </si>
-  <si>
-    <t>loss_model2</t>
-  </si>
-  <si>
-    <t>loss_model3</t>
-  </si>
-  <si>
-    <t>loss_model4</t>
-  </si>
-  <si>
-    <t>loss_model_laf</t>
   </si>
   <si>
     <t>model1</t>
@@ -122,38 +107,7 @@
     </mc:Fallback>
   </mc:AlternateContent>
   <c:chart>
-    <c:title>
-      <c:layout/>
-      <c:overlay val="0"/>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-      </c:spPr>
-      <c:txPr>
-        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr>
-            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="65000"/>
-                  <a:lumOff val="35000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:pPr>
-          <a:endParaRPr lang="en-US"/>
-        </a:p>
-      </c:txPr>
-    </c:title>
-    <c:autoTitleDeleted val="0"/>
+    <c:autoTitleDeleted val="1"/>
     <c:plotArea>
       <c:layout/>
       <c:scatterChart>
@@ -168,7 +122,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>loss_model1</c:v>
+                  <c:v>model1</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -183,7 +137,19 @@
             <a:effectLst/>
           </c:spPr>
           <c:marker>
-            <c:symbol val="none"/>
+            <c:symbol val="square"/>
+            <c:size val="2"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
           </c:marker>
           <c:xVal>
             <c:numRef>
@@ -519,7 +485,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>loss_model2</c:v>
+                  <c:v>model2</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -534,7 +500,19 @@
             <a:effectLst/>
           </c:spPr>
           <c:marker>
-            <c:symbol val="none"/>
+            <c:symbol val="triangle"/>
+            <c:size val="2"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent2"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
           </c:marker>
           <c:xVal>
             <c:numRef>
@@ -870,7 +848,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>loss_model3</c:v>
+                  <c:v>model3</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -878,14 +856,26 @@
           <c:spPr>
             <a:ln w="19050" cap="rnd">
               <a:solidFill>
-                <a:schemeClr val="accent3"/>
+                <a:schemeClr val="accent5"/>
               </a:solidFill>
               <a:round/>
             </a:ln>
             <a:effectLst/>
           </c:spPr>
           <c:marker>
-            <c:symbol val="none"/>
+            <c:symbol val="diamond"/>
+            <c:size val="2"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent5"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent5"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
           </c:marker>
           <c:xVal>
             <c:numRef>
@@ -1221,7 +1211,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>loss_model4</c:v>
+                  <c:v>model4</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -1236,7 +1226,17 @@
             <a:effectLst/>
           </c:spPr>
           <c:marker>
-            <c:symbol val="none"/>
+            <c:symbol val="x"/>
+            <c:size val="2"/>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent4"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
           </c:marker>
           <c:xVal>
             <c:numRef>
@@ -1596,6 +1596,32 @@
           </c:spPr>
         </c:majorGridlines>
         <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1200" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:sysClr val="windowText" lastClr="000000"/>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US" sz="1200">
+                    <a:solidFill>
+                      <a:sysClr val="windowText" lastClr="000000"/>
+                    </a:solidFill>
+                  </a:rPr>
+                  <a:t>Epoch</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
           <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
@@ -1610,12 +1636,9 @@
             <a:lstStyle/>
             <a:p>
               <a:pPr>
-                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:defRPr sz="1200" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                   <a:solidFill>
-                    <a:schemeClr val="tx1">
-                      <a:lumMod val="65000"/>
-                      <a:lumOff val="35000"/>
-                    </a:schemeClr>
+                    <a:sysClr val="windowText" lastClr="000000"/>
                   </a:solidFill>
                   <a:latin typeface="+mn-lt"/>
                   <a:ea typeface="+mn-ea"/>
@@ -1648,7 +1671,7 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:defRPr sz="1100" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                 <a:solidFill>
                   <a:schemeClr val="tx1">
                     <a:lumMod val="65000"/>
@@ -1689,6 +1712,32 @@
           </c:spPr>
         </c:majorGridlines>
         <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1200" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:sysClr val="windowText" lastClr="000000"/>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US" sz="1200">
+                    <a:solidFill>
+                      <a:sysClr val="windowText" lastClr="000000"/>
+                    </a:solidFill>
+                  </a:rPr>
+                  <a:t>Loss</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
           <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
@@ -1703,12 +1752,9 @@
             <a:lstStyle/>
             <a:p>
               <a:pPr>
-                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:defRPr sz="1200" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                   <a:solidFill>
-                    <a:schemeClr val="tx1">
-                      <a:lumMod val="65000"/>
-                      <a:lumOff val="35000"/>
-                    </a:schemeClr>
+                    <a:sysClr val="windowText" lastClr="000000"/>
                   </a:solidFill>
                   <a:latin typeface="+mn-lt"/>
                   <a:ea typeface="+mn-ea"/>
@@ -1741,7 +1787,7 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:defRPr sz="1100" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                 <a:solidFill>
                   <a:schemeClr val="tx1">
                     <a:lumMod val="65000"/>
@@ -1851,38 +1897,7 @@
     </mc:Fallback>
   </mc:AlternateContent>
   <c:chart>
-    <c:title>
-      <c:layout/>
-      <c:overlay val="0"/>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-      </c:spPr>
-      <c:txPr>
-        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr>
-            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="65000"/>
-                  <a:lumOff val="35000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:pPr>
-          <a:endParaRPr lang="en-US"/>
-        </a:p>
-      </c:txPr>
-    </c:title>
-    <c:autoTitleDeleted val="0"/>
+    <c:autoTitleDeleted val="1"/>
     <c:plotArea>
       <c:layout/>
       <c:scatterChart>
@@ -1897,7 +1912,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>loss_model1</c:v>
+                  <c:v>model1</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -1912,7 +1927,19 @@
             <a:effectLst/>
           </c:spPr>
           <c:marker>
-            <c:symbol val="none"/>
+            <c:symbol val="square"/>
+            <c:size val="2"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
           </c:marker>
           <c:xVal>
             <c:numRef>
@@ -2248,7 +2275,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>loss_model2</c:v>
+                  <c:v>model2</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -2263,7 +2290,19 @@
             <a:effectLst/>
           </c:spPr>
           <c:marker>
-            <c:symbol val="none"/>
+            <c:symbol val="triangle"/>
+            <c:size val="2"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent2"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
           </c:marker>
           <c:xVal>
             <c:numRef>
@@ -2599,7 +2638,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>loss_model3</c:v>
+                  <c:v>model3</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -2607,14 +2646,26 @@
           <c:spPr>
             <a:ln w="19050" cap="rnd">
               <a:solidFill>
-                <a:schemeClr val="accent3"/>
+                <a:schemeClr val="accent5"/>
               </a:solidFill>
               <a:round/>
             </a:ln>
             <a:effectLst/>
           </c:spPr>
           <c:marker>
-            <c:symbol val="none"/>
+            <c:symbol val="diamond"/>
+            <c:size val="2"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent5"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent5"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
           </c:marker>
           <c:xVal>
             <c:numRef>
@@ -2950,7 +3001,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>loss_model4</c:v>
+                  <c:v>model4</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -2965,7 +3016,17 @@
             <a:effectLst/>
           </c:spPr>
           <c:marker>
-            <c:symbol val="none"/>
+            <c:symbol val="x"/>
+            <c:size val="2"/>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent4"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
           </c:marker>
           <c:xVal>
             <c:numRef>
@@ -3301,7 +3362,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>loss_model_laf</c:v>
+                  <c:v>model_laf</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -3309,14 +3370,26 @@
           <c:spPr>
             <a:ln w="19050" cap="rnd">
               <a:solidFill>
-                <a:schemeClr val="accent5"/>
+                <a:srgbClr val="7030A0"/>
               </a:solidFill>
               <a:round/>
             </a:ln>
             <a:effectLst/>
           </c:spPr>
           <c:marker>
-            <c:symbol val="none"/>
+            <c:symbol val="circle"/>
+            <c:size val="2"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="7030A0"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:srgbClr val="7030A0"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
           </c:marker>
           <c:xVal>
             <c:numRef>
@@ -3675,6 +3748,60 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1200" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:sysClr val="windowText" lastClr="000000"/>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US" sz="1200">
+                    <a:solidFill>
+                      <a:sysClr val="windowText" lastClr="000000"/>
+                    </a:solidFill>
+                  </a:rPr>
+                  <a:t>Epoch</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1200" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:sysClr val="windowText" lastClr="000000"/>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
@@ -3697,7 +3824,7 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:defRPr sz="1100" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                 <a:solidFill>
                   <a:schemeClr val="tx1">
                     <a:lumMod val="65000"/>
@@ -3737,6 +3864,60 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1200" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:sysClr val="windowText" lastClr="000000"/>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US" sz="1200">
+                    <a:solidFill>
+                      <a:sysClr val="windowText" lastClr="000000"/>
+                    </a:solidFill>
+                  </a:rPr>
+                  <a:t>Loss</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1200" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:sysClr val="windowText" lastClr="000000"/>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
@@ -3759,7 +3940,7 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:defRPr sz="1100" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                 <a:solidFill>
                   <a:schemeClr val="tx1">
                     <a:lumMod val="65000"/>
@@ -3856,6 +4037,1075 @@
 </file>
 
 <file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="1"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>training_loss!$C$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>model2</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="triangle"/>
+            <c:size val="4"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent2"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>training_loss!$A$2:$A$51</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="50"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>13</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>14</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>17</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>18</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>19</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>21</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>22</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>23</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>24</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>25</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>26</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>27</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>28</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>29</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>30</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>31</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>32</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>33</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>34</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>35</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>36</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>37</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>38</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>39</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>40</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>41</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>42</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>43</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>44</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>45</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>46</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>47</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>48</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>49</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>training_loss!$C$2:$C$51</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="50"/>
+                <c:pt idx="0">
+                  <c:v>0.53977590242645201</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.39780772505971101</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.37294860535204399</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.36004987057823301</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.35276969143070902</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.34868357642565201</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.34843543768360302</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.34570577303428102</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.33578361148116898</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.33659996643232198</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.33730880252050899</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0.33084903960352802</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>0.33047803750202398</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>0.33368461616077999</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>0.321205856382828</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>0.325864946095763</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>0.32844917785098898</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>0.32574474269301501</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>0.32015105348950601</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>0.32577452783483901</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>0.31958495055755098</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>0.316766177703806</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>0.30969722092758201</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>0.323082927211993</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>0.31343665082567201</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>0.32274366212828198</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>0.31644859991553997</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>0.318995431795631</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>0.31649128946500699</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>0.31465612766932199</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>0.31275328795696</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>0.31481203712450401</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>0.31258451600661302</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>0.31786878110901001</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>0.31300616390844999</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>0.31295310098659401</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>0.31130532590233401</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>0.31465692709286602</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>0.31180855702536697</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>0.30398318501931199</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>0.30639388156435798</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>0.29842804139639201</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>0.305501834697472</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>0.30585484765483301</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>0.306089557859133</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>0.31183399826709401</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>0.30577777044538401</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>0.30452479873019001</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>0.313088851813694</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>0.30845228104394201</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-67B7-48CF-805E-0E3015FC7F5A}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>training_loss!$F$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>model_laf</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="bg1">
+                  <a:lumMod val="50000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="4"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="bg1">
+                  <a:lumMod val="50000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="bg1">
+                    <a:lumMod val="50000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>training_loss!$A$2:$A$51</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="50"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>13</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>14</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>17</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>18</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>19</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>21</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>22</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>23</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>24</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>25</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>26</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>27</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>28</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>29</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>30</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>31</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>32</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>33</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>34</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>35</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>36</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>37</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>38</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>39</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>40</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>41</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>42</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>43</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>44</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>45</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>46</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>47</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>48</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>49</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>training_loss!$F$2:$F$51</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="50"/>
+                <c:pt idx="0">
+                  <c:v>3.22122277188467</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2.67211942623018</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2.3905474229264798</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2.1687851860415299</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1.97779093746227</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1.80962378989398</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1.6697530458655301</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1.5536961013623201</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>1.4565942663659299</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>1.3741455809691701</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>1.3058001542383699</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>1.2467223697218901</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>1.19690354770373</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>1.1512713928854701</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>1.1113563864768601</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>1.07606612169724</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>1.0436938745257001</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>1.0151742954331799</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>0.98849146296291601</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>0.96376463638728604</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>0.94092958810846505</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>0.92034475754185896</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>0.90091085272801796</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>0.88355418037349798</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>0.86660990002861604</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>0.85043165874453697</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>0.83536831097348896</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>0.82160526299399395</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>0.80783132577810002</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>0.795859870313815</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>0.78418050325787503</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>0.77332798582960405</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>0.76228412965647596</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>0.75151445987851895</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>0.74162586601998304</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>0.73264886348041502</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>0.72443492291657596</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>0.71571038247099505</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>0.70679906745152399</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>0.69838906549305002</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>0.69165180391796699</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>0.68406764799556796</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>0.67715427067053602</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>0.67035251353153202</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>0.66411149237897604</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>0.65743837681833905</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>0.65105884272071202</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>0.64522765749080402</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>0.63942553457044704</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>0.63293163488339699</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-67B7-48CF-805E-0E3015FC7F5A}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="547983535"/>
+        <c:axId val="547985199"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="547983535"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1200" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:sysClr val="windowText" lastClr="000000"/>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US" sz="1200">
+                    <a:solidFill>
+                      <a:sysClr val="windowText" lastClr="000000"/>
+                    </a:solidFill>
+                  </a:rPr>
+                  <a:t>Epoch</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1200" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:sysClr val="windowText" lastClr="000000"/>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1100" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="547985199"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="547985199"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1200" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:sysClr val="windowText" lastClr="000000"/>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US" sz="1200">
+                    <a:solidFill>
+                      <a:sysClr val="windowText" lastClr="000000"/>
+                    </a:solidFill>
+                  </a:rPr>
+                  <a:t>Loss</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1200" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:sysClr val="windowText" lastClr="000000"/>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1100" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="547983535"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1200" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup paperSize="9" orientation="landscape"/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
@@ -5873,7 +7123,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart5.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
@@ -7700,6 +8950,46 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors5.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
   <cs:axisTitle>
@@ -9764,20 +11054,536 @@
 </cs:chartStyle>
 </file>
 
+<file path=xl/charts/style5.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>10</xdr:col>
-      <xdr:colOff>171450</xdr:colOff>
-      <xdr:row>3</xdr:row>
-      <xdr:rowOff>85725</xdr:rowOff>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>485775</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>133350</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>18</xdr:col>
-      <xdr:colOff>590550</xdr:colOff>
-      <xdr:row>26</xdr:row>
-      <xdr:rowOff>142875</xdr:rowOff>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>39375</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>134850</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -9798,20 +11604,52 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>10</xdr:col>
-      <xdr:colOff>180974</xdr:colOff>
-      <xdr:row>27</xdr:row>
-      <xdr:rowOff>114300</xdr:rowOff>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>485774</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>38103</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>18</xdr:col>
-      <xdr:colOff>609599</xdr:colOff>
-      <xdr:row>45</xdr:row>
-      <xdr:rowOff>19050</xdr:rowOff>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>39374</xdr:colOff>
+      <xdr:row>35</xdr:row>
+      <xdr:rowOff>39603</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
         <xdr:cNvPr id="3" name="Chart 2"/>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>490536</xdr:colOff>
+      <xdr:row>35</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>590549</xdr:colOff>
+      <xdr:row>50</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="4" name="Chart 3"/>
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
@@ -9820,7 +11658,7 @@
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
-          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId3"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -10159,8 +11997,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F51"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="I6" sqref="I6"/>
+    <sheetView tabSelected="1" topLeftCell="A10" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="J53" sqref="J53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -10180,16 +12018,16 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D1" t="s">
+        <v>4</v>
+      </c>
+      <c r="E1" t="s">
+        <v>5</v>
+      </c>
+      <c r="F1" t="s">
         <v>2</v>
-      </c>
-      <c r="D1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" t="s">
-        <v>4</v>
-      </c>
-      <c r="F1" t="s">
-        <v>5</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
@@ -11205,7 +13043,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F51"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="T17" sqref="T17"/>
     </sheetView>
   </sheetViews>
@@ -11223,19 +13061,19 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="C1" t="s">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="D1" t="s">
-        <v>9</v>
+        <v>4</v>
       </c>
       <c r="E1" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="F1" t="s">
-        <v>7</v>
+        <v>2</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">

</xml_diff>